<commit_message>
Finished resolved rates and contact detection, wrote a readme.md
</commit_message>
<xml_diff>
--- a/MATLAB/haoran_model/Joint_Kinematics.xlsx
+++ b/MATLAB/haoran_model/Joint_Kinematics.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="6036"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v1_arm_urdf" sheetId="2" r:id="rId1"/>
+    <sheet name="necessity_v1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+  <si>
+    <t>Joint #</t>
+  </si>
   <si>
     <t>Parent #</t>
   </si>
@@ -33,6 +37,21 @@
     <t>fixed</t>
   </si>
   <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
     <t>Link #</t>
   </si>
   <si>
@@ -66,6 +85,12 @@
     <t>V1_arm1_pitch_a_link</t>
   </si>
   <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
     <t>V1_arm1_pitch_b_link</t>
   </si>
   <si>
@@ -94,6 +119,45 @@
   </si>
   <si>
     <t>V1_arm1_RCM_link</t>
+  </si>
+  <si>
+    <t>common_robot_frame</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>q9</t>
+  </si>
+  <si>
+    <t>q10</t>
+  </si>
+  <si>
+    <t>q11</t>
+  </si>
+  <si>
+    <t>q13</t>
+  </si>
+  <si>
+    <t>q12</t>
+  </si>
+  <si>
+    <t>rcm joint angle</t>
   </si>
 </sst>
 </file>
@@ -109,12 +173,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,8 +199,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,25 +482,530 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -440,13 +1016,16 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -454,297 +1033,368 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
         <v>8</v>
       </c>
-      <c r="D10">
-        <v>-7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>-7</v>
       </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
         <v>14</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>14</v>
       </c>
       <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>3</v>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>